<commit_message>
Project 1 with macro Completed
</commit_message>
<xml_diff>
--- a/Project - 1/InsertingAndFormattingText.xlsx
+++ b/Project - 1/InsertingAndFormattingText.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Excel-Projects\Project - 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6377DC5-04D7-4C4C-AEF7-17E09A061E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C106A94-2018-414A-A553-61E2CFCF43B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EAST RECORDS" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +119,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -147,9 +153,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -228,7 +233,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="41148" rIns="45720" bIns="41148" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="36576" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -520,7 +525,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A3:I18"/>
+  <dimension ref="A3:F18"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:F18"/>
@@ -533,324 +538,323 @@
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>45658</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>45689</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>45717</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>45748</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>800</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>650</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>700</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>2150</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>900</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>850</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>850</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>2600</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>4850</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>3200</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1155</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>9205</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1250</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1250</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1250</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>3750</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2025</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>2200</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1650</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>5875</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1350</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>1500</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>1700</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>4550</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>3300</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>3500</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>3700</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>10500</v>
       </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>3825</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>3725</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>3750</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>11300</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>8900</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>10315</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>5250</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>24465</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>6250</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>6000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>6500</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>18750</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>8000</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>8000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>8000</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>24000</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>11500</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>12500</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>12500</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>36500</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>12250</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>12250</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>12750</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>37250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>25000</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>24000</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>26390</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>75390</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <f>SUM(C4:C17)</f>
         <v>90200</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <f>SUM(D4:D17)</f>
         <v>89940</v>
       </c>
-      <c r="E18" s="2">
-        <f t="shared" ref="D18:F18" si="0">SUM(E4:E17)</f>
+      <c r="E18" s="1">
+        <f t="shared" ref="E18:F18" si="0">SUM(E4:E17)</f>
         <v>86145</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>266285</v>
       </c>
@@ -875,322 +879,322 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>45658</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>45689</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>45717</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>45748</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>800</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>650</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>700</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>2150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>900</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>850</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>850</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>2600</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>4850</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>3200</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1155</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>9205</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1250</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1250</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1250</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>3750</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2025</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>2200</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1650</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>5875</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1350</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>1500</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>1700</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>4550</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>3300</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>3500</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>3700</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>10500</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>3825</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>3725</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>3750</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>11300</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>8900</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>10315</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>5250</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>24465</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>6250</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>6000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>6500</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>18750</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>8000</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>8000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>8000</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>24000</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>11500</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>12500</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>12500</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>36500</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>12250</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>12250</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>12750</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>37250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>25000</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>24000</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>26390</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>75390</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <f>SUM(C4:C17)</f>
         <v>90200</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <f>SUM(D4:D17)</f>
         <v>89940</v>
       </c>
-      <c r="E18" s="2">
-        <f t="shared" ref="D18:F18" si="0">SUM(E4:E17)</f>
+      <c r="E18" s="1">
+        <f t="shared" ref="E18:F18" si="0">SUM(E4:E17)</f>
         <v>86145</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>266285</v>
       </c>
@@ -1205,8 +1209,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:F18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="99" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,322 +1219,322 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>45658</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>45689</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>45717</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>45748</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>800</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>650</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>700</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>2150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>900</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>850</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>850</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>2600</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>4850</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>3200</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1155</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>9205</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1250</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1250</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1250</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>3750</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2025</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>2200</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1650</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>5875</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>1350</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>1500</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>1700</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>4550</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>3300</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>3500</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>3700</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>10500</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>3825</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>3725</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>3750</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>11300</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>8900</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>10315</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>5250</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>24465</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>6250</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>6000</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>6500</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>18750</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>8000</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>8000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>8000</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>24000</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>11500</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>12500</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>12500</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>36500</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>12250</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>12250</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>12750</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>37250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>25000</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>24000</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>26390</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>75390</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <f>SUM(C4:C17)</f>
         <v>90200</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <f>SUM(D4:D17)</f>
         <v>89940</v>
       </c>
-      <c r="E18" s="2">
-        <f t="shared" ref="D18:F18" si="0">SUM(E4:E17)</f>
+      <c r="E18" s="1">
+        <f t="shared" ref="E18:F18" si="0">SUM(E4:E17)</f>
         <v>86145</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <f t="shared" si="0"/>
         <v>266285</v>
       </c>

</xml_diff>